<commit_message>
added docs and spreadsheet for motor feedback analysis
</commit_message>
<xml_diff>
--- a/firmware/motor control.xlsx
+++ b/firmware/motor control.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>pid_output_left</t>
   </si>
@@ -58,19 +58,53 @@
   </si>
   <si>
     <t>THEN set output 3 high for a forward direction</t>
+  </si>
+  <si>
+    <t>left_motor</t>
+  </si>
+  <si>
+    <t>period</t>
+  </si>
+  <si>
+    <t>freq</t>
+  </si>
+  <si>
+    <t>angle(deg)</t>
+  </si>
+  <si>
+    <t>deg/sec</t>
+  </si>
+  <si>
+    <t>rot/sec</t>
+  </si>
+  <si>
+    <t>in/sec</t>
+  </si>
+  <si>
+    <t>time to correct</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>ft/min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="3">
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -109,17 +143,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -150,79 +196,82 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>pid_corrected</c:v>
+          </c:tx>
           <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$C$15:$C$33</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>-400.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-200.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-100.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-50.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-25.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-20.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-15.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-10.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-5.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>15.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>20.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>25.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>50.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>100.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>200.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>400.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$D$15:$D$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
+                  <c:v>-400.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-200.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-100.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-50.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-25.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-20.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-15.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-10.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-5.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>400.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$15:$E$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
                   <c:v>-391.5525672371638</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -278,6 +327,146 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>391.5525672371638</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>motor_control</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$15:$D$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>-400.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-200.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-100.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-50.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-25.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-20.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-15.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-10.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-5.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>400.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$15:$F$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>-8.447432762836172</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-21.31578947368422</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-45.45871559633031</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-88.22033898305085</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-156.7647058823529</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-184.6551724137931</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-224.1666666666667</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-284.4736842105263</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-387.8571428571428</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>387.8571428571428</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>284.4736842105263</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>224.1666666666667</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>184.6551724137931</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>156.7647058823529</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>88.22033898305085</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>45.45871559633031</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>21.31578947368422</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.447432762836172</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -292,11 +481,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2051357496"/>
-        <c:axId val="-2051670616"/>
+        <c:axId val="-2134187224"/>
+        <c:axId val="2082305240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2051357496"/>
+        <c:axId val="-2134187224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -326,12 +515,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2051670616"/>
+        <c:crossAx val="2082305240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2051670616"/>
+        <c:axId val="2082305240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -361,7 +550,276 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2051357496"/>
+        <c:crossAx val="-2134187224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>motor_control</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$15:$C$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>-26.66666666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-13.33333333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-6.666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-3.333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1.666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1.333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-1.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13.33333333333333</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>26.66666666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$15:$F$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>-8.447432762836172</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-21.31578947368422</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-45.45871559633031</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-88.22033898305085</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-156.7647058823529</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-184.6551724137931</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-224.1666666666667</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-284.4736842105263</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-387.8571428571428</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>387.8571428571428</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>284.4736842105263</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>224.1666666666667</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>184.6551724137931</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>156.7647058823529</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>88.22033898305085</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>45.45871559633031</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>21.31578947368422</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.447432762836172</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2095506776"/>
+        <c:axId val="-2095511656"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2095506776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>angle</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2095511656"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2095511656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Corrected</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2095506776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -382,16 +840,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -405,6 +863,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -735,249 +1225,955 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:D33"/>
+  <dimension ref="C1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:4">
-      <c r="C1" t="s">
+    <row r="1" spans="3:13">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="3:4">
-      <c r="C2" t="s">
+    <row r="2" spans="3:13">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="3:4">
-      <c r="C3" t="s">
+    <row r="3" spans="3:13">
+      <c r="D3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="3:4">
-      <c r="C4" t="s">
+    <row r="4" spans="3:13">
+      <c r="D4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="3:4">
-      <c r="C5" t="s">
+    <row r="5" spans="3:13">
+      <c r="D5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="3:4">
-      <c r="C6" t="s">
+    <row r="6" spans="3:13">
+      <c r="D6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="3:4">
-      <c r="C7" t="s">
+    <row r="7" spans="3:13">
+      <c r="D7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="3:4">
-      <c r="C8" t="s">
+    <row r="8" spans="3:13">
+      <c r="D8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="3:4">
-      <c r="C9" t="s">
+    <row r="9" spans="3:13">
+      <c r="D9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="3:4">
-      <c r="C10" t="s">
+    <row r="10" spans="3:13">
+      <c r="D10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="3:4">
-      <c r="C11" t="s">
+    <row r="11" spans="3:13">
+      <c r="D11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="3:4">
+    <row r="13" spans="3:13">
+      <c r="M13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="3:13">
       <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" t="s">
         <v>0</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="3:4">
-      <c r="C15">
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L14" t="s">
+        <v>22</v>
+      </c>
+      <c r="M14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="3:13">
+      <c r="C15" s="4">
+        <f>D15/15</f>
+        <v>-26.666666666666668</v>
+      </c>
+      <c r="D15">
         <v>-400</v>
       </c>
-      <c r="D15">
-        <f>(-405)-(1/(C15-9))*5500</f>
+      <c r="E15">
+        <f>(-405)-(1/(D15-9))*5500</f>
         <v>-391.55256723716383</v>
       </c>
-    </row>
-    <row r="16" spans="3:4">
-      <c r="C16">
+      <c r="F15">
+        <f t="shared" ref="F15:F22" si="0">-400-E15</f>
+        <v>-8.4474327628361721</v>
+      </c>
+      <c r="G15">
+        <f>F15*0.00004</f>
+        <v>-3.3789731051344691E-4</v>
+      </c>
+      <c r="H15" s="1">
+        <f>1/G15</f>
+        <v>-2959.4790159189624</v>
+      </c>
+      <c r="I15" s="3">
+        <f>H15/200/4</f>
+        <v>-3.6993487698987031</v>
+      </c>
+      <c r="J15" s="1">
+        <f>I15*360</f>
+        <v>-1331.765557163533</v>
+      </c>
+      <c r="K15" s="4">
+        <f>I15*PI()*90/25.4</f>
+        <v>-41.179772546150325</v>
+      </c>
+      <c r="L15" s="4">
+        <f>K15/12*60</f>
+        <v>-205.89886273075163</v>
+      </c>
+      <c r="M15" s="2">
+        <f>C15/J15*1000</f>
+        <v>20.023544326722785</v>
+      </c>
+    </row>
+    <row r="16" spans="3:13">
+      <c r="C16" s="4">
+        <f t="shared" ref="C16:C33" si="1">D16/15</f>
+        <v>-13.333333333333334</v>
+      </c>
+      <c r="D16">
         <v>-200</v>
       </c>
-      <c r="D16">
-        <f t="shared" ref="D16:D23" si="0">(-405)-(1/(C16-9))*5500</f>
+      <c r="E16">
+        <f t="shared" ref="E16:E23" si="2">(-405)-(1/(D16-9))*5500</f>
         <v>-378.68421052631578</v>
       </c>
-    </row>
-    <row r="17" spans="3:4">
-      <c r="C17">
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>-21.31578947368422</v>
+      </c>
+      <c r="G16">
+        <f t="shared" ref="G16:G33" si="3">F16*0.00004</f>
+        <v>-8.5263157894736885E-4</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" ref="H16:H23" si="4">1/G16</f>
+        <v>-1172.8395061728388</v>
+      </c>
+      <c r="I16" s="3">
+        <f t="shared" ref="I16:I33" si="5">H16/200/4</f>
+        <v>-1.4660493827160486</v>
+      </c>
+      <c r="J16" s="1">
+        <f t="shared" ref="J16:J33" si="6">I16*360</f>
+        <v>-527.77777777777749</v>
+      </c>
+      <c r="K16" s="4">
+        <f>I16*PI()*90/25.4</f>
+        <v>-16.319515643647758</v>
+      </c>
+      <c r="L16" s="4">
+        <f t="shared" ref="L16:L33" si="7">K16/12*60</f>
+        <v>-81.597578218238795</v>
+      </c>
+      <c r="M16" s="2">
+        <f>C16/J16*1000</f>
+        <v>25.263157894736857</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13">
+      <c r="C17" s="4">
+        <f t="shared" si="1"/>
+        <v>-6.666666666666667</v>
+      </c>
+      <c r="D17">
         <v>-100</v>
       </c>
-      <c r="D17">
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>-354.54128440366969</v>
+      </c>
+      <c r="F17">
         <f t="shared" si="0"/>
-        <v>-354.54128440366969</v>
-      </c>
-    </row>
-    <row r="18" spans="3:4">
-      <c r="C18">
+        <v>-45.458715596330308</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="3"/>
+        <v>-1.8183486238532124E-3</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="4"/>
+        <v>-549.94954591321857</v>
+      </c>
+      <c r="I17" s="3">
+        <f t="shared" si="5"/>
+        <v>-0.68743693239152326</v>
+      </c>
+      <c r="J17" s="1">
+        <f t="shared" si="6"/>
+        <v>-247.47729566094839</v>
+      </c>
+      <c r="K17" s="4">
+        <f>I17*PI()*90/25.4</f>
+        <v>-7.6522918698691393</v>
+      </c>
+      <c r="L17" s="4">
+        <f t="shared" si="7"/>
+        <v>-38.261459349345699</v>
+      </c>
+      <c r="M17" s="2">
+        <f>C17/J17*1000</f>
+        <v>26.938498131158699</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13">
+      <c r="C18" s="4">
+        <f t="shared" si="1"/>
+        <v>-3.3333333333333335</v>
+      </c>
+      <c r="D18">
         <v>-50</v>
       </c>
-      <c r="D18">
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>-311.77966101694915</v>
+      </c>
+      <c r="F18">
         <f t="shared" si="0"/>
-        <v>-311.77966101694915</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4">
-      <c r="C19">
+        <v>-88.220338983050851</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="3"/>
+        <v>-3.5288135593220344E-3</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="4"/>
+        <v>-283.38136407300669</v>
+      </c>
+      <c r="I18" s="3">
+        <f t="shared" si="5"/>
+        <v>-0.35422670509125836</v>
+      </c>
+      <c r="J18" s="1">
+        <f t="shared" si="6"/>
+        <v>-127.52161383285301</v>
+      </c>
+      <c r="K18" s="4">
+        <f>I18*PI()*90/25.4</f>
+        <v>-3.9431197361339128</v>
+      </c>
+      <c r="L18" s="4">
+        <f t="shared" si="7"/>
+        <v>-19.715598680669562</v>
+      </c>
+      <c r="M18" s="2">
+        <f>C18/J18*1000</f>
+        <v>26.139359698681737</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13">
+      <c r="C19" s="4">
+        <f t="shared" si="1"/>
+        <v>-1.6666666666666667</v>
+      </c>
+      <c r="D19">
         <v>-25</v>
       </c>
-      <c r="D19">
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>-243.23529411764707</v>
+      </c>
+      <c r="F19">
         <f t="shared" si="0"/>
-        <v>-243.23529411764707</v>
-      </c>
-    </row>
-    <row r="20" spans="3:4">
-      <c r="C20">
+        <v>-156.76470588235293</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="3"/>
+        <v>-6.2705882352941172E-3</v>
+      </c>
+      <c r="H19" s="1">
+        <f t="shared" si="4"/>
+        <v>-159.47467166979362</v>
+      </c>
+      <c r="I19" s="3">
+        <f t="shared" si="5"/>
+        <v>-0.19934333958724204</v>
+      </c>
+      <c r="J19" s="1">
+        <f t="shared" si="6"/>
+        <v>-71.763602251407136</v>
+      </c>
+      <c r="K19" s="4">
+        <f>I19*PI()*90/25.4</f>
+        <v>-2.2190158034267773</v>
+      </c>
+      <c r="L19" s="4">
+        <f t="shared" si="7"/>
+        <v>-11.095079017133887</v>
+      </c>
+      <c r="M19" s="2">
+        <f>C19/J19*1000</f>
+        <v>23.224400871459697</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13">
+      <c r="C20" s="4">
+        <f t="shared" si="1"/>
+        <v>-1.3333333333333333</v>
+      </c>
+      <c r="D20">
         <v>-20</v>
       </c>
-      <c r="D20">
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>-215.34482758620689</v>
+      </c>
+      <c r="F20">
         <f t="shared" si="0"/>
-        <v>-215.34482758620689</v>
-      </c>
-    </row>
-    <row r="21" spans="3:4">
-      <c r="C21">
+        <v>-184.65517241379311</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="3"/>
+        <v>-7.3862068965517254E-3</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" si="4"/>
+        <v>-135.38748832866477</v>
+      </c>
+      <c r="I20" s="3">
+        <f t="shared" si="5"/>
+        <v>-0.16923436041083095</v>
+      </c>
+      <c r="J20" s="1">
+        <f t="shared" si="6"/>
+        <v>-60.924369747899142</v>
+      </c>
+      <c r="K20" s="4">
+        <f>I20*PI()*90/25.4</f>
+        <v>-1.883853862446734</v>
+      </c>
+      <c r="L20" s="4">
+        <f t="shared" si="7"/>
+        <v>-9.4192693122336699</v>
+      </c>
+      <c r="M20" s="2">
+        <f>C20/J20*1000</f>
+        <v>21.885057471264375</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13">
+      <c r="C21" s="4">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="D21">
         <v>-15</v>
       </c>
-      <c r="D21">
+      <c r="E21">
+        <f t="shared" si="2"/>
+        <v>-175.83333333333334</v>
+      </c>
+      <c r="F21">
         <f t="shared" si="0"/>
-        <v>-175.83333333333334</v>
-      </c>
-    </row>
-    <row r="22" spans="3:4">
-      <c r="C22">
+        <v>-224.16666666666666</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="3"/>
+        <v>-8.9666666666666662E-3</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" si="4"/>
+        <v>-111.52416356877325</v>
+      </c>
+      <c r="I21" s="3">
+        <f t="shared" si="5"/>
+        <v>-0.13940520446096655</v>
+      </c>
+      <c r="J21" s="1">
+        <f t="shared" si="6"/>
+        <v>-50.185873605947954</v>
+      </c>
+      <c r="K21" s="4">
+        <f>I21*PI()*90/25.4</f>
+        <v>-1.5518068093940158</v>
+      </c>
+      <c r="L21" s="4">
+        <f t="shared" si="7"/>
+        <v>-7.75903404697008</v>
+      </c>
+      <c r="M21" s="2">
+        <f>C21/J21*1000</f>
+        <v>19.925925925925927</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13">
+      <c r="C22" s="4">
+        <f t="shared" si="1"/>
+        <v>-0.66666666666666663</v>
+      </c>
+      <c r="D22">
         <v>-10</v>
       </c>
-      <c r="D22">
+      <c r="E22">
+        <f t="shared" si="2"/>
+        <v>-115.5263157894737</v>
+      </c>
+      <c r="F22">
         <f t="shared" si="0"/>
-        <v>-115.5263157894737</v>
-      </c>
-    </row>
-    <row r="23" spans="3:4">
-      <c r="C23">
+        <v>-284.4736842105263</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="3"/>
+        <v>-1.1378947368421053E-2</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" si="4"/>
+        <v>-87.881591119333947</v>
+      </c>
+      <c r="I22" s="3">
+        <f t="shared" si="5"/>
+        <v>-0.10985198889916743</v>
+      </c>
+      <c r="J22" s="1">
+        <f t="shared" si="6"/>
+        <v>-39.546716003700276</v>
+      </c>
+      <c r="K22" s="4">
+        <f>I22*PI()*90/25.4</f>
+        <v>-1.2228314219569556</v>
+      </c>
+      <c r="L22" s="4">
+        <f t="shared" si="7"/>
+        <v>-6.1141571097847782</v>
+      </c>
+      <c r="M22" s="2">
+        <f>C22/J22*1000</f>
+        <v>16.857699805068229</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13">
+      <c r="C23" s="4">
+        <f t="shared" si="1"/>
+        <v>-0.33333333333333331</v>
+      </c>
+      <c r="D23">
         <v>-5</v>
       </c>
-      <c r="D23">
-        <f t="shared" si="0"/>
+      <c r="E23">
+        <f t="shared" si="2"/>
         <v>-12.142857142857167</v>
       </c>
-    </row>
-    <row r="24" spans="3:4">
-      <c r="C24">
+      <c r="F23">
+        <f>-400-E23</f>
+        <v>-387.85714285714283</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="3"/>
+        <v>-1.5514285714285715E-2</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" si="4"/>
+        <v>-64.456721915285442</v>
+      </c>
+      <c r="I23" s="3">
+        <f t="shared" si="5"/>
+        <v>-8.0570902394106803E-2</v>
+      </c>
+      <c r="J23" s="1">
+        <f t="shared" si="6"/>
+        <v>-29.005524861878449</v>
+      </c>
+      <c r="K23" s="4">
+        <f>I23*PI()*90/25.4</f>
+        <v>-0.89688527381489602</v>
+      </c>
+      <c r="L23" s="4">
+        <f t="shared" si="7"/>
+        <v>-4.4844263690744794</v>
+      </c>
+      <c r="M23" s="2">
+        <f>C23/J23*1000</f>
+        <v>11.492063492063492</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13">
+      <c r="C24" s="4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D24">
-        <f>C24</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="3:4">
-      <c r="C25">
+      <c r="E24">
+        <f>D24</f>
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="I24" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="4">
+        <f>I24*PI()*90/25.4</f>
+        <v>0</v>
+      </c>
+      <c r="L24" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M24" s="2"/>
+    </row>
+    <row r="25" spans="3:13">
+      <c r="C25" s="4">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D25">
         <v>5</v>
       </c>
-      <c r="D25">
-        <f t="shared" ref="D25:D30" si="1">(405)-(1/(C25+9))*5500</f>
+      <c r="E25">
+        <f t="shared" ref="E25:E30" si="8">(405)-(1/(D25+9))*5500</f>
         <v>12.142857142857167</v>
       </c>
-    </row>
-    <row r="26" spans="3:4">
-      <c r="C26">
+      <c r="F25">
+        <f>400-E25</f>
+        <v>387.85714285714283</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="3"/>
+        <v>1.5514285714285715E-2</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" ref="H25:H33" si="9">1/G25</f>
+        <v>64.456721915285442</v>
+      </c>
+      <c r="I25" s="3">
+        <f t="shared" si="5"/>
+        <v>8.0570902394106803E-2</v>
+      </c>
+      <c r="J25" s="1">
+        <f t="shared" si="6"/>
+        <v>29.005524861878449</v>
+      </c>
+      <c r="K25" s="4">
+        <f>I25*PI()*90/25.4</f>
+        <v>0.89688527381489602</v>
+      </c>
+      <c r="L25" s="4">
+        <f t="shared" si="7"/>
+        <v>4.4844263690744794</v>
+      </c>
+      <c r="M25" s="2">
+        <f>C25/J25*1000</f>
+        <v>11.492063492063492</v>
+      </c>
+    </row>
+    <row r="26" spans="3:13">
+      <c r="C26" s="4">
+        <f t="shared" si="1"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D26">
         <v>10</v>
       </c>
-      <c r="D26">
+      <c r="E26">
+        <f t="shared" si="8"/>
+        <v>115.5263157894737</v>
+      </c>
+      <c r="F26">
+        <f t="shared" ref="F26:F33" si="10">400-E26</f>
+        <v>284.4736842105263</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="3"/>
+        <v>1.1378947368421053E-2</v>
+      </c>
+      <c r="H26" s="1">
+        <f t="shared" si="9"/>
+        <v>87.881591119333947</v>
+      </c>
+      <c r="I26" s="3">
+        <f t="shared" si="5"/>
+        <v>0.10985198889916743</v>
+      </c>
+      <c r="J26" s="1">
+        <f t="shared" si="6"/>
+        <v>39.546716003700276</v>
+      </c>
+      <c r="K26" s="4">
+        <f>I26*PI()*90/25.4</f>
+        <v>1.2228314219569556</v>
+      </c>
+      <c r="L26" s="4">
+        <f t="shared" si="7"/>
+        <v>6.1141571097847782</v>
+      </c>
+      <c r="M26" s="2">
+        <f>C26/J26*1000</f>
+        <v>16.857699805068229</v>
+      </c>
+    </row>
+    <row r="27" spans="3:13">
+      <c r="C27" s="4">
         <f t="shared" si="1"/>
-        <v>115.5263157894737</v>
-      </c>
-    </row>
-    <row r="27" spans="3:4">
-      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
         <v>15</v>
       </c>
-      <c r="D27">
+      <c r="E27">
+        <f t="shared" si="8"/>
+        <v>175.83333333333334</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="10"/>
+        <v>224.16666666666666</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="3"/>
+        <v>8.9666666666666662E-3</v>
+      </c>
+      <c r="H27" s="1">
+        <f t="shared" si="9"/>
+        <v>111.52416356877325</v>
+      </c>
+      <c r="I27" s="3">
+        <f t="shared" si="5"/>
+        <v>0.13940520446096655</v>
+      </c>
+      <c r="J27" s="1">
+        <f t="shared" si="6"/>
+        <v>50.185873605947954</v>
+      </c>
+      <c r="K27" s="4">
+        <f>I27*PI()*90/25.4</f>
+        <v>1.5518068093940158</v>
+      </c>
+      <c r="L27" s="4">
+        <f t="shared" si="7"/>
+        <v>7.75903404697008</v>
+      </c>
+      <c r="M27" s="2">
+        <f>C27/J27*1000</f>
+        <v>19.925925925925927</v>
+      </c>
+    </row>
+    <row r="28" spans="3:13">
+      <c r="C28" s="4">
         <f t="shared" si="1"/>
-        <v>175.83333333333334</v>
-      </c>
-    </row>
-    <row r="28" spans="3:4">
-      <c r="C28">
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="D28">
         <v>20</v>
       </c>
-      <c r="D28">
+      <c r="E28">
+        <f t="shared" si="8"/>
+        <v>215.34482758620689</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="10"/>
+        <v>184.65517241379311</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="3"/>
+        <v>7.3862068965517254E-3</v>
+      </c>
+      <c r="H28" s="1">
+        <f t="shared" si="9"/>
+        <v>135.38748832866477</v>
+      </c>
+      <c r="I28" s="3">
+        <f t="shared" si="5"/>
+        <v>0.16923436041083095</v>
+      </c>
+      <c r="J28" s="1">
+        <f t="shared" si="6"/>
+        <v>60.924369747899142</v>
+      </c>
+      <c r="K28" s="4">
+        <f>I28*PI()*90/25.4</f>
+        <v>1.883853862446734</v>
+      </c>
+      <c r="L28" s="4">
+        <f t="shared" si="7"/>
+        <v>9.4192693122336699</v>
+      </c>
+      <c r="M28" s="2">
+        <f>C28/J28*1000</f>
+        <v>21.885057471264375</v>
+      </c>
+    </row>
+    <row r="29" spans="3:13">
+      <c r="C29" s="4">
         <f t="shared" si="1"/>
-        <v>215.34482758620689</v>
-      </c>
-    </row>
-    <row r="29" spans="3:4">
-      <c r="C29">
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="D29">
         <v>25</v>
       </c>
-      <c r="D29">
+      <c r="E29">
+        <f t="shared" si="8"/>
+        <v>243.23529411764707</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="10"/>
+        <v>156.76470588235293</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="3"/>
+        <v>6.2705882352941172E-3</v>
+      </c>
+      <c r="H29" s="1">
+        <f t="shared" si="9"/>
+        <v>159.47467166979362</v>
+      </c>
+      <c r="I29" s="3">
+        <f t="shared" si="5"/>
+        <v>0.19934333958724204</v>
+      </c>
+      <c r="J29" s="1">
+        <f t="shared" si="6"/>
+        <v>71.763602251407136</v>
+      </c>
+      <c r="K29" s="4">
+        <f>I29*PI()*90/25.4</f>
+        <v>2.2190158034267773</v>
+      </c>
+      <c r="L29" s="4">
+        <f t="shared" si="7"/>
+        <v>11.095079017133887</v>
+      </c>
+      <c r="M29" s="2">
+        <f>C29/J29*1000</f>
+        <v>23.224400871459697</v>
+      </c>
+    </row>
+    <row r="30" spans="3:13">
+      <c r="C30" s="4">
         <f t="shared" si="1"/>
-        <v>243.23529411764707</v>
-      </c>
-    </row>
-    <row r="30" spans="3:4">
-      <c r="C30">
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="D30">
         <v>50</v>
       </c>
-      <c r="D30">
+      <c r="E30">
+        <f t="shared" si="8"/>
+        <v>311.77966101694915</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="10"/>
+        <v>88.220338983050851</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="3"/>
+        <v>3.5288135593220344E-3</v>
+      </c>
+      <c r="H30" s="1">
+        <f t="shared" si="9"/>
+        <v>283.38136407300669</v>
+      </c>
+      <c r="I30" s="3">
+        <f t="shared" si="5"/>
+        <v>0.35422670509125836</v>
+      </c>
+      <c r="J30" s="1">
+        <f t="shared" si="6"/>
+        <v>127.52161383285301</v>
+      </c>
+      <c r="K30" s="4">
+        <f>I30*PI()*90/25.4</f>
+        <v>3.9431197361339128</v>
+      </c>
+      <c r="L30" s="4">
+        <f t="shared" si="7"/>
+        <v>19.715598680669562</v>
+      </c>
+      <c r="M30" s="2">
+        <f>C30/J30*1000</f>
+        <v>26.139359698681737</v>
+      </c>
+    </row>
+    <row r="31" spans="3:13">
+      <c r="C31" s="4">
         <f t="shared" si="1"/>
-        <v>311.77966101694915</v>
-      </c>
-    </row>
-    <row r="31" spans="3:4">
-      <c r="C31">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="D31">
         <v>100</v>
       </c>
-      <c r="D31">
-        <f>(405)-(1/(C31+9))*5500</f>
+      <c r="E31">
+        <f>(405)-(1/(D31+9))*5500</f>
         <v>354.54128440366969</v>
       </c>
-    </row>
-    <row r="32" spans="3:4">
-      <c r="C32">
+      <c r="F31">
+        <f t="shared" si="10"/>
+        <v>45.458715596330308</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="3"/>
+        <v>1.8183486238532124E-3</v>
+      </c>
+      <c r="H31" s="1">
+        <f t="shared" si="9"/>
+        <v>549.94954591321857</v>
+      </c>
+      <c r="I31" s="3">
+        <f t="shared" si="5"/>
+        <v>0.68743693239152326</v>
+      </c>
+      <c r="J31" s="1">
+        <f t="shared" si="6"/>
+        <v>247.47729566094839</v>
+      </c>
+      <c r="K31" s="4">
+        <f>I31*PI()*90/25.4</f>
+        <v>7.6522918698691393</v>
+      </c>
+      <c r="L31" s="4">
+        <f t="shared" si="7"/>
+        <v>38.261459349345699</v>
+      </c>
+      <c r="M31" s="2">
+        <f>C31/J31*1000</f>
+        <v>26.938498131158699</v>
+      </c>
+    </row>
+    <row r="32" spans="3:13">
+      <c r="C32" s="4">
+        <f t="shared" si="1"/>
+        <v>13.333333333333334</v>
+      </c>
+      <c r="D32">
         <v>200</v>
       </c>
-      <c r="D32">
-        <f t="shared" ref="D32:D33" si="2">(405)-(1/(C32+9))*5500</f>
+      <c r="E32">
+        <f t="shared" ref="E32:E33" si="11">(405)-(1/(D32+9))*5500</f>
         <v>378.68421052631578</v>
       </c>
-    </row>
-    <row r="33" spans="3:4">
-      <c r="C33">
+      <c r="F32">
+        <f t="shared" si="10"/>
+        <v>21.31578947368422</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="3"/>
+        <v>8.5263157894736885E-4</v>
+      </c>
+      <c r="H32" s="1">
+        <f t="shared" si="9"/>
+        <v>1172.8395061728388</v>
+      </c>
+      <c r="I32" s="3">
+        <f t="shared" si="5"/>
+        <v>1.4660493827160486</v>
+      </c>
+      <c r="J32" s="1">
+        <f t="shared" si="6"/>
+        <v>527.77777777777749</v>
+      </c>
+      <c r="K32" s="4">
+        <f>I32*PI()*90/25.4</f>
+        <v>16.319515643647758</v>
+      </c>
+      <c r="L32" s="4">
+        <f t="shared" si="7"/>
+        <v>81.597578218238795</v>
+      </c>
+      <c r="M32" s="2">
+        <f>C32/J32*1000</f>
+        <v>25.263157894736857</v>
+      </c>
+    </row>
+    <row r="33" spans="3:13">
+      <c r="C33" s="4">
+        <f t="shared" si="1"/>
+        <v>26.666666666666668</v>
+      </c>
+      <c r="D33">
         <v>400</v>
       </c>
-      <c r="D33">
-        <f t="shared" si="2"/>
+      <c r="E33">
+        <f t="shared" si="11"/>
         <v>391.55256723716383</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="10"/>
+        <v>8.4474327628361721</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="3"/>
+        <v>3.3789731051344691E-4</v>
+      </c>
+      <c r="H33" s="1">
+        <f t="shared" si="9"/>
+        <v>2959.4790159189624</v>
+      </c>
+      <c r="I33" s="3">
+        <f t="shared" si="5"/>
+        <v>3.6993487698987031</v>
+      </c>
+      <c r="J33" s="1">
+        <f t="shared" si="6"/>
+        <v>1331.765557163533</v>
+      </c>
+      <c r="K33" s="4">
+        <f>I33*PI()*90/25.4</f>
+        <v>41.179772546150325</v>
+      </c>
+      <c r="L33" s="4">
+        <f t="shared" si="7"/>
+        <v>205.89886273075163</v>
+      </c>
+      <c r="M33" s="2">
+        <f>C33/J33*1000</f>
+        <v>20.023544326722785</v>
       </c>
     </row>
   </sheetData>

</xml_diff>